<commit_message>
Checks and fixes of charging strategies with many trucks and limited grid cap
- fixed flickering behavior due to counting available capacity
- fixed listing errors in MAX_POWER chargign
- adjusted input files (no fixed charging profile, more vehicles and smaller grid connection)
</commit_message>
<xml_diff>
--- a/Base/inputTruckTripPatterns.xlsx
+++ b/Base/inputTruckTripPatterns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/p_hogeveen_tue_nl/Documents/HOLON/Base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{43749885-E160-4C11-ABE5-5990E1AC7E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A24F4FBE-7B26-45A0-8359-693F17E2C8E0}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="8_{43749885-E160-4C11-ABE5-5990E1AC7E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FABBCEB-D803-47FF-964F-1A295CC983E3}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="795" windowWidth="24450" windowHeight="11385" xr2:uid="{668C4D5B-BF80-4C89-92DD-46FB23AE2C30}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{668C4D5B-BF80-4C89-92DD-46FB23AE2C30}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -54,34 +54,25 @@
     <t>6_16_300km</t>
   </si>
   <si>
-    <t>6_16_400km</t>
-  </si>
-  <si>
-    <t>6_16_500km</t>
-  </si>
-  <si>
     <t>6_17_250km</t>
   </si>
   <si>
     <t>6_17_300km</t>
   </si>
   <si>
-    <t>6_17_400km</t>
-  </si>
-  <si>
-    <t>6_17_500km</t>
-  </si>
-  <si>
     <t>6_18.5_300km</t>
   </si>
   <si>
-    <t>6_18.5_400km</t>
-  </si>
-  <si>
-    <t>6_18.5_500km</t>
-  </si>
-  <si>
     <t>nb_trips</t>
+  </si>
+  <si>
+    <t>6.5_18.25_280km</t>
+  </si>
+  <si>
+    <t>6_18_250km</t>
+  </si>
+  <si>
+    <t>6.5_19.5_340km</t>
   </si>
 </sst>
 </file>
@@ -433,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1320E17-0C62-4F56-BE78-D069AA2D3497}">
-  <dimension ref="A1:W12"/>
+  <dimension ref="A1:W9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,7 +441,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -660,55 +651,55 @@
         <v>300</v>
       </c>
       <c r="D4">
-        <v>960</v>
+        <v>1020</v>
       </c>
       <c r="E4">
-        <v>388</v>
+        <v>258</v>
       </c>
       <c r="F4">
         <v>1800</v>
       </c>
       <c r="G4">
-        <v>2400</v>
+        <v>2460</v>
       </c>
       <c r="H4">
-        <v>391</v>
+        <v>269</v>
       </c>
       <c r="I4">
-        <v>3240</v>
+        <v>3180</v>
       </c>
       <c r="J4">
-        <v>3840</v>
+        <v>3900</v>
       </c>
       <c r="K4">
-        <v>394</v>
+        <v>263</v>
       </c>
       <c r="L4">
-        <v>4680</v>
+        <v>4620</v>
       </c>
       <c r="M4">
-        <v>5280</v>
+        <v>5340</v>
       </c>
       <c r="N4">
-        <v>399</v>
+        <v>249</v>
       </c>
       <c r="O4">
-        <v>6120</v>
+        <v>6060</v>
       </c>
       <c r="P4">
-        <v>6720</v>
+        <v>6780</v>
       </c>
       <c r="Q4">
-        <v>423</v>
+        <v>231</v>
       </c>
       <c r="R4">
         <v>7560</v>
       </c>
       <c r="S4">
-        <v>8160</v>
+        <v>8220</v>
       </c>
       <c r="T4">
-        <v>405</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
@@ -716,70 +707,61 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>360</v>
       </c>
       <c r="D5">
-        <v>960</v>
+        <v>1020</v>
       </c>
       <c r="E5">
-        <v>513</v>
+        <v>314</v>
       </c>
       <c r="F5">
-        <v>1860</v>
+        <v>1800</v>
       </c>
       <c r="G5">
-        <v>2400</v>
+        <v>2460</v>
       </c>
       <c r="H5">
-        <v>480</v>
+        <v>292</v>
       </c>
       <c r="I5">
-        <v>3240</v>
+        <v>3300</v>
       </c>
       <c r="J5">
-        <v>3840</v>
+        <v>3900</v>
       </c>
       <c r="K5">
-        <v>505</v>
+        <v>297</v>
       </c>
       <c r="L5">
-        <v>4740</v>
+        <v>4680</v>
       </c>
       <c r="M5">
-        <v>5280</v>
+        <v>5340</v>
       </c>
       <c r="N5">
-        <v>482</v>
+        <v>309</v>
       </c>
       <c r="O5">
-        <v>6120</v>
+        <v>6180</v>
       </c>
       <c r="P5">
-        <v>6720</v>
+        <v>6780</v>
       </c>
       <c r="Q5">
-        <v>483</v>
+        <v>298</v>
       </c>
       <c r="R5">
         <v>7620</v>
       </c>
       <c r="S5">
-        <v>8160</v>
+        <v>8220</v>
       </c>
       <c r="T5">
-        <v>521</v>
-      </c>
-      <c r="U5">
-        <v>9000</v>
-      </c>
-      <c r="V5">
-        <v>9600</v>
-      </c>
-      <c r="W5">
-        <v>508</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -790,125 +772,134 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>300</v>
+        <v>360</v>
       </c>
       <c r="D6">
-        <v>1020</v>
+        <v>1080</v>
       </c>
       <c r="E6">
-        <v>258</v>
+        <v>296</v>
       </c>
       <c r="F6">
         <v>1800</v>
       </c>
       <c r="G6">
-        <v>2460</v>
+        <v>2520</v>
       </c>
       <c r="H6">
-        <v>269</v>
+        <v>310</v>
       </c>
       <c r="I6">
-        <v>3180</v>
+        <v>3240</v>
       </c>
       <c r="J6">
-        <v>3900</v>
+        <v>4020</v>
       </c>
       <c r="K6">
-        <v>263</v>
+        <v>299</v>
       </c>
       <c r="L6">
         <v>4620</v>
       </c>
       <c r="M6">
-        <v>5340</v>
+        <v>5400</v>
       </c>
       <c r="N6">
-        <v>249</v>
+        <v>298</v>
       </c>
       <c r="O6">
-        <v>6060</v>
+        <v>6120</v>
       </c>
       <c r="P6">
-        <v>6780</v>
+        <v>6900</v>
       </c>
       <c r="Q6">
-        <v>231</v>
+        <v>310</v>
       </c>
       <c r="R6">
         <v>7560</v>
       </c>
       <c r="S6">
-        <v>8220</v>
+        <v>8340</v>
       </c>
       <c r="T6">
-        <v>233</v>
+        <v>317</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>360</v>
       </c>
       <c r="D7">
-        <v>1020</v>
+        <v>1080</v>
       </c>
       <c r="E7">
-        <v>314</v>
+        <v>291</v>
       </c>
       <c r="F7">
         <v>1800</v>
       </c>
       <c r="G7">
-        <v>2460</v>
+        <v>2520</v>
       </c>
       <c r="H7">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="I7">
         <v>3300</v>
       </c>
       <c r="J7">
-        <v>3900</v>
+        <v>3960</v>
       </c>
       <c r="K7">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="L7">
         <v>4680</v>
       </c>
       <c r="M7">
-        <v>5340</v>
+        <v>5400</v>
       </c>
       <c r="N7">
-        <v>309</v>
+        <v>265</v>
       </c>
       <c r="O7">
-        <v>6180</v>
+        <v>6120</v>
       </c>
       <c r="P7">
-        <v>6780</v>
+        <v>6840</v>
       </c>
       <c r="Q7">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="R7">
-        <v>7620</v>
+        <v>7560</v>
       </c>
       <c r="S7">
-        <v>8220</v>
+        <v>8280</v>
       </c>
       <c r="T7">
-        <v>282</v>
+        <v>268</v>
+      </c>
+      <c r="U7">
+        <v>9000</v>
+      </c>
+      <c r="V7">
+        <v>9720</v>
+      </c>
+      <c r="W7">
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -917,330 +908,126 @@
         <v>360</v>
       </c>
       <c r="D8">
-        <v>1020</v>
+        <v>1080</v>
       </c>
       <c r="E8">
-        <v>387</v>
+        <v>230</v>
       </c>
       <c r="F8">
         <v>1800</v>
       </c>
       <c r="G8">
-        <v>2460</v>
+        <v>2520</v>
       </c>
       <c r="H8">
-        <v>411</v>
+        <v>235</v>
       </c>
       <c r="I8">
-        <v>3300</v>
+        <v>3240</v>
       </c>
       <c r="J8">
-        <v>3900</v>
+        <v>3960</v>
       </c>
       <c r="K8">
-        <v>395</v>
+        <v>241</v>
       </c>
       <c r="L8">
         <v>4680</v>
       </c>
       <c r="M8">
-        <v>5340</v>
+        <v>5400</v>
       </c>
       <c r="N8">
-        <v>409</v>
+        <v>276</v>
       </c>
       <c r="O8">
         <v>6120</v>
       </c>
       <c r="P8">
-        <v>6780</v>
+        <v>6840</v>
       </c>
       <c r="Q8">
-        <v>403</v>
+        <v>250</v>
       </c>
       <c r="R8">
         <v>7560</v>
       </c>
       <c r="S8">
-        <v>8220</v>
+        <v>8280</v>
       </c>
       <c r="T8">
-        <v>392</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>7</v>
       </c>
       <c r="C9">
-        <v>360</v>
+        <v>420</v>
       </c>
       <c r="D9">
-        <v>1020</v>
+        <v>1140</v>
       </c>
       <c r="E9">
-        <v>526</v>
+        <v>330</v>
       </c>
       <c r="F9">
         <v>1800</v>
       </c>
       <c r="G9">
-        <v>2460</v>
+        <v>2640</v>
       </c>
       <c r="H9">
-        <v>476</v>
+        <v>323</v>
       </c>
       <c r="I9">
         <v>3300</v>
       </c>
       <c r="J9">
-        <v>3900</v>
+        <v>4080</v>
       </c>
       <c r="K9">
-        <v>523</v>
+        <v>355</v>
       </c>
       <c r="L9">
-        <v>4680</v>
+        <v>4740</v>
       </c>
       <c r="M9">
-        <v>5340</v>
+        <v>5460</v>
       </c>
       <c r="N9">
-        <v>481</v>
+        <v>335</v>
       </c>
       <c r="O9">
-        <v>6180</v>
+        <v>6120</v>
       </c>
       <c r="P9">
-        <v>6780</v>
+        <v>6960</v>
       </c>
       <c r="Q9">
-        <v>472</v>
+        <v>327</v>
       </c>
       <c r="R9">
-        <v>7560</v>
+        <v>7620</v>
       </c>
       <c r="S9">
-        <v>8220</v>
+        <v>8400</v>
       </c>
       <c r="T9">
-        <v>513</v>
+        <v>328</v>
       </c>
       <c r="U9">
-        <v>9060</v>
+        <v>9000</v>
       </c>
       <c r="V9">
-        <v>9660</v>
+        <v>9840</v>
       </c>
       <c r="W9">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10">
-        <v>6</v>
-      </c>
-      <c r="C10">
-        <v>360</v>
-      </c>
-      <c r="D10">
-        <v>1080</v>
-      </c>
-      <c r="E10">
-        <v>296</v>
-      </c>
-      <c r="F10">
-        <v>1800</v>
-      </c>
-      <c r="G10">
-        <v>2520</v>
-      </c>
-      <c r="H10">
-        <v>310</v>
-      </c>
-      <c r="I10">
-        <v>3240</v>
-      </c>
-      <c r="J10">
-        <v>4020</v>
-      </c>
-      <c r="K10">
-        <v>299</v>
-      </c>
-      <c r="L10">
-        <v>4620</v>
-      </c>
-      <c r="M10">
-        <v>5400</v>
-      </c>
-      <c r="N10">
-        <v>298</v>
-      </c>
-      <c r="O10">
-        <v>6120</v>
-      </c>
-      <c r="P10">
-        <v>6900</v>
-      </c>
-      <c r="Q10">
-        <v>310</v>
-      </c>
-      <c r="R10">
-        <v>7560</v>
-      </c>
-      <c r="S10">
-        <v>8340</v>
-      </c>
-      <c r="T10">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11">
-        <v>7</v>
-      </c>
-      <c r="C11">
-        <v>300</v>
-      </c>
-      <c r="D11">
-        <v>1080</v>
-      </c>
-      <c r="E11">
-        <v>391</v>
-      </c>
-      <c r="F11">
-        <v>1740</v>
-      </c>
-      <c r="G11">
-        <v>2580</v>
-      </c>
-      <c r="H11">
-        <v>408</v>
-      </c>
-      <c r="I11">
-        <v>3240</v>
-      </c>
-      <c r="J11">
-        <v>3960</v>
-      </c>
-      <c r="K11">
-        <v>421</v>
-      </c>
-      <c r="L11">
-        <v>4680</v>
-      </c>
-      <c r="M11">
-        <v>5460</v>
-      </c>
-      <c r="N11">
-        <v>395</v>
-      </c>
-      <c r="O11">
-        <v>6060</v>
-      </c>
-      <c r="P11">
-        <v>6840</v>
-      </c>
-      <c r="Q11">
-        <v>417</v>
-      </c>
-      <c r="R11">
-        <v>7560</v>
-      </c>
-      <c r="S11">
-        <v>8340</v>
-      </c>
-      <c r="T11">
-        <v>398</v>
-      </c>
-      <c r="U11">
-        <v>9060</v>
-      </c>
-      <c r="V11">
-        <v>9720</v>
-      </c>
-      <c r="W11">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12">
-        <v>7</v>
-      </c>
-      <c r="C12">
-        <v>360</v>
-      </c>
-      <c r="D12">
-        <v>1080</v>
-      </c>
-      <c r="E12">
-        <v>517</v>
-      </c>
-      <c r="F12">
-        <v>1860</v>
-      </c>
-      <c r="G12">
-        <v>2520</v>
-      </c>
-      <c r="H12">
-        <v>481</v>
-      </c>
-      <c r="I12">
-        <v>3180</v>
-      </c>
-      <c r="J12">
-        <v>4020</v>
-      </c>
-      <c r="K12">
-        <v>469</v>
-      </c>
-      <c r="L12">
-        <v>4680</v>
-      </c>
-      <c r="M12">
-        <v>5400</v>
-      </c>
-      <c r="N12">
-        <v>466</v>
-      </c>
-      <c r="O12">
-        <v>6120</v>
-      </c>
-      <c r="P12">
-        <v>6840</v>
-      </c>
-      <c r="Q12">
-        <v>472</v>
-      </c>
-      <c r="R12">
-        <v>7560</v>
-      </c>
-      <c r="S12">
-        <v>8280</v>
-      </c>
-      <c r="T12">
-        <v>478</v>
-      </c>
-      <c r="U12">
-        <v>9000</v>
-      </c>
-      <c r="V12">
-        <v>9780</v>
-      </c>
-      <c r="W12">
-        <v>496</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Electric cooking for households start
Added cooking hob trackers to model cooking behavior similar to trucks
</commit_message>
<xml_diff>
--- a/Base/inputTruckTripPatterns.xlsx
+++ b/Base/inputTruckTripPatterns.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/p_hogeveen_tue_nl/Documents/HOLON/Base/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20180652\OneDrive - TU Eindhoven\Documents\GitHub\Holon\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="8_{43749885-E160-4C11-ABE5-5990E1AC7E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FABBCEB-D803-47FF-964F-1A295CC983E3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F68207-BC32-46A4-89F1-B998F073E578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{668C4D5B-BF80-4C89-92DD-46FB23AE2C30}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>6.5_19.5_340km</t>
+  </si>
+  <si>
+    <t>10% zon</t>
+  </si>
+  <si>
+    <t>30% zat</t>
   </si>
 </sst>
 </file>
@@ -424,15 +430,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1320E17-0C62-4F56-BE78-D069AA2D3497}">
-  <dimension ref="A1:W9"/>
+  <dimension ref="A1:W13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1030,6 +1037,16 @@
         <v>350</v>
       </c>
     </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>